<commit_message>
Prep for revision 1
</commit_message>
<xml_diff>
--- a/stats/estimation_stats.xlsx
+++ b/stats/estimation_stats.xlsx
@@ -1,41 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="front" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref1_forced_licks" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref1_latency" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref1_auc" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref1_free_licks" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref1_choices" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref2_forced_licks_nr" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref2_latency_nr" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref2_free_licks_nr" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref2_choices_nr" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref2_auc_nr" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref3_forced_licks_nr" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref3_latency_nr" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref3_free_licks_nr" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref3_choices_nr" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref3_auc_nr" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref2_forced_licks_pr" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref2_latency_pr" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref2_free_licks_pr" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref2_choices_pr" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref2_auc_pr" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref3_forced_licks_pr" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref3_latency_pr" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref3_free_licks_pr" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref3_choices_pr" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pref3_auc_pr" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="summary_nr" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="summary_pr" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="summary_auc_nr" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="summary_auc_pr" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="front" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="pref1_forced_licks" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="pref1_latency" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="pref1_auc" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="pref1_free_licks" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="pref1_choices" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="pref2_forced_licks_nr" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="pref2_latency_nr" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="pref2_free_licks_nr" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="pref2_choices_nr" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="pref2_auc_nr" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="pref3_forced_licks_nr" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="pref3_latency_nr" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="pref3_free_licks_nr" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="pref3_choices_nr" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="pref3_auc_nr" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="pref2_forced_licks_pr" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="pref2_latency_pr" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="pref2_free_licks_pr" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="pref2_choices_pr" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="pref2_auc_pr" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="pref3_forced_licks_pr" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="pref3_latency_pr" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="pref3_free_licks_pr" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="pref3_choices_pr" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="pref3_auc_pr" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="summary_nr" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="summary_pr" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="summary_auc_nr" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="summary_auc_pr" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="pref1_lateauc" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="pref1_lateauc1" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="pref1_lateauc2" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="pref1_lateauc3" sheetId="34" state="visible" r:id="rId34"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -73,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -103,23 +107,100 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="4">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -663,7 +744,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -885,7 +966,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -1108,7 +1189,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -1331,7 +1412,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -1554,7 +1635,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -1777,7 +1858,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -1999,7 +2080,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -2222,7 +2303,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -2445,7 +2526,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -2668,7 +2749,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -2891,7 +2972,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -3201,7 +3282,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -3424,7 +3505,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -3647,7 +3728,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -3870,7 +3951,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -4093,7 +4174,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -4316,7 +4397,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -4539,7 +4620,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -4762,7 +4843,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -5092,7 +5173,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -5424,7 +5505,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -5756,7 +5837,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -6066,7 +6147,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -6398,7 +6479,1247 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>control</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>control_N</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>test_N</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>effect_size</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>is_paired</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>difference</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>ci</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>bca_low</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>bca_high</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>bca_interval_idx</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>pct_low</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>pct_high</t>
+        </is>
+      </c>
+      <c r="O1" s="3" t="inlineStr">
+        <is>
+          <t>pct_interval_idx</t>
+        </is>
+      </c>
+      <c r="P1" s="3" t="inlineStr">
+        <is>
+          <t>bootstraps</t>
+        </is>
+      </c>
+      <c r="Q1" s="3" t="inlineStr">
+        <is>
+          <t>resamples</t>
+        </is>
+      </c>
+      <c r="R1" s="3" t="inlineStr">
+        <is>
+          <t>random_seed</t>
+        </is>
+      </c>
+      <c r="S1" s="3" t="inlineStr">
+        <is>
+          <t>pvalue_permutation</t>
+        </is>
+      </c>
+      <c r="T1" s="3" t="inlineStr">
+        <is>
+          <t>permutation_count</t>
+        </is>
+      </c>
+      <c r="U1" s="3" t="inlineStr">
+        <is>
+          <t>pvalue_wilcoxon</t>
+        </is>
+      </c>
+      <c r="V1" s="3" t="inlineStr">
+        <is>
+          <t>statistic_wilcoxon</t>
+        </is>
+      </c>
+      <c r="W1" s="3" t="inlineStr">
+        <is>
+          <t>pvalue_paired_students_t</t>
+        </is>
+      </c>
+      <c r="X1" s="3" t="inlineStr">
+        <is>
+          <t>statistic_paired_students_t</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>control1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>mean difference</t>
+        </is>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.181398634009704</v>
+      </c>
+      <c r="I2" t="n">
+        <v>95</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.6080379091540522</v>
+      </c>
+      <c r="K2" t="n">
+        <v>2.535525662759842</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>(74, 4810)</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>-0.4407462515386924</v>
+      </c>
+      <c r="N2" t="n">
+        <v>2.658289886448642</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>(125, 4875)</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>[-1.80529007 -1.80529007 -1.67246845 ...  3.45470257  3.58752419
+  3.66338636]</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="R2" t="n">
+        <v>12345</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.2252</v>
+      </c>
+      <c r="T2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.3125</v>
+      </c>
+      <c r="V2" t="n">
+        <v>5</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.2255779037553131</v>
+      </c>
+      <c r="X2" t="n">
+        <v>-1.381818993572075</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>control2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>test2</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>mean difference</t>
+        </is>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.8396280075262637</v>
+      </c>
+      <c r="I3" t="n">
+        <v>95</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-0.7019448623986144</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3.5002453177765</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>(258, 4956)</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>-0.9379203764316902</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2.978988898899568</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>(125, 4875)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>[-2.24695086 -2.04684412 -2.00907616 ...  4.70365302  5.09968474
+  5.33792856]</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v>5000</v>
+      </c>
+      <c r="R3" t="n">
+        <v>12345</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.5154</v>
+      </c>
+      <c r="T3" t="n">
+        <v>5000</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.65234375</v>
+      </c>
+      <c r="V3" t="n">
+        <v>18</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.4604991813964153</v>
+      </c>
+      <c r="X3" t="n">
+        <v>-0.7752356862657116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>control</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>control_N</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>test_N</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>effect_size</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>is_paired</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>difference</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>ci</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>bca_low</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>bca_high</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>bca_interval_idx</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>pct_low</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>pct_high</t>
+        </is>
+      </c>
+      <c r="O1" s="3" t="inlineStr">
+        <is>
+          <t>pct_interval_idx</t>
+        </is>
+      </c>
+      <c r="P1" s="3" t="inlineStr">
+        <is>
+          <t>bootstraps</t>
+        </is>
+      </c>
+      <c r="Q1" s="3" t="inlineStr">
+        <is>
+          <t>resamples</t>
+        </is>
+      </c>
+      <c r="R1" s="3" t="inlineStr">
+        <is>
+          <t>random_seed</t>
+        </is>
+      </c>
+      <c r="S1" s="3" t="inlineStr">
+        <is>
+          <t>pvalue_permutation</t>
+        </is>
+      </c>
+      <c r="T1" s="3" t="inlineStr">
+        <is>
+          <t>permutation_count</t>
+        </is>
+      </c>
+      <c r="U1" s="3" t="inlineStr">
+        <is>
+          <t>pvalue_wilcoxon</t>
+        </is>
+      </c>
+      <c r="V1" s="3" t="inlineStr">
+        <is>
+          <t>statistic_wilcoxon</t>
+        </is>
+      </c>
+      <c r="W1" s="3" t="inlineStr">
+        <is>
+          <t>pvalue_paired_students_t</t>
+        </is>
+      </c>
+      <c r="X1" s="3" t="inlineStr">
+        <is>
+          <t>statistic_paired_students_t</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>control1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>mean difference</t>
+        </is>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.181398634009704</v>
+      </c>
+      <c r="I2" t="n">
+        <v>95</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.6080379091540522</v>
+      </c>
+      <c r="K2" t="n">
+        <v>2.535525662759842</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>(74, 4810)</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>-0.4407462515386924</v>
+      </c>
+      <c r="N2" t="n">
+        <v>2.658289886448642</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>(125, 4875)</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>[-1.80529007 -1.80529007 -1.67246845 ...  3.45470257  3.58752419
+  3.66338636]</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="R2" t="n">
+        <v>12345</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.2252</v>
+      </c>
+      <c r="T2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.3125</v>
+      </c>
+      <c r="V2" t="n">
+        <v>5</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.2255779037553131</v>
+      </c>
+      <c r="X2" t="n">
+        <v>-1.381818993572075</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>control2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>test2</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>mean difference</t>
+        </is>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.8396280075262637</v>
+      </c>
+      <c r="I3" t="n">
+        <v>95</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-0.7019448623986144</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3.5002453177765</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>(258, 4956)</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>-0.9379203764316902</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2.978988898899568</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>(125, 4875)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>[-2.24695086 -2.04684412 -2.00907616 ...  4.70365302  5.09968474
+  5.33792856]</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v>5000</v>
+      </c>
+      <c r="R3" t="n">
+        <v>12345</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.5154</v>
+      </c>
+      <c r="T3" t="n">
+        <v>5000</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.65234375</v>
+      </c>
+      <c r="V3" t="n">
+        <v>18</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.4604991813964153</v>
+      </c>
+      <c r="X3" t="n">
+        <v>-0.7752356862657116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>control</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>control_N</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>test_N</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>effect_size</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>is_paired</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>difference</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>ci</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>bca_low</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>bca_high</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>bca_interval_idx</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>pct_low</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>pct_high</t>
+        </is>
+      </c>
+      <c r="O1" s="3" t="inlineStr">
+        <is>
+          <t>pct_interval_idx</t>
+        </is>
+      </c>
+      <c r="P1" s="3" t="inlineStr">
+        <is>
+          <t>bootstraps</t>
+        </is>
+      </c>
+      <c r="Q1" s="3" t="inlineStr">
+        <is>
+          <t>resamples</t>
+        </is>
+      </c>
+      <c r="R1" s="3" t="inlineStr">
+        <is>
+          <t>random_seed</t>
+        </is>
+      </c>
+      <c r="S1" s="3" t="inlineStr">
+        <is>
+          <t>pvalue_permutation</t>
+        </is>
+      </c>
+      <c r="T1" s="3" t="inlineStr">
+        <is>
+          <t>permutation_count</t>
+        </is>
+      </c>
+      <c r="U1" s="3" t="inlineStr">
+        <is>
+          <t>pvalue_wilcoxon</t>
+        </is>
+      </c>
+      <c r="V1" s="3" t="inlineStr">
+        <is>
+          <t>statistic_wilcoxon</t>
+        </is>
+      </c>
+      <c r="W1" s="3" t="inlineStr">
+        <is>
+          <t>pvalue_paired_students_t</t>
+        </is>
+      </c>
+      <c r="X1" s="3" t="inlineStr">
+        <is>
+          <t>statistic_paired_students_t</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>control1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>mean difference</t>
+        </is>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.181398634009704</v>
+      </c>
+      <c r="I2" t="n">
+        <v>95</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.6080379091540522</v>
+      </c>
+      <c r="K2" t="n">
+        <v>2.535525662759842</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>(74, 4810)</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>-0.4407462515386924</v>
+      </c>
+      <c r="N2" t="n">
+        <v>2.658289886448642</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>(125, 4875)</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>[-1.80529007 -1.80529007 -1.67246845 ...  3.45470257  3.58752419
+  3.66338636]</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="R2" t="n">
+        <v>12345</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.2252</v>
+      </c>
+      <c r="T2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.3125</v>
+      </c>
+      <c r="V2" t="n">
+        <v>5</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.2255779037553131</v>
+      </c>
+      <c r="X2" t="n">
+        <v>-1.381818993572075</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>control2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>test2</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>mean difference</t>
+        </is>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.8396280075262637</v>
+      </c>
+      <c r="I3" t="n">
+        <v>95</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-0.7019448623986144</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3.5002453177765</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>(258, 4956)</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>-0.9379203764316902</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2.978988898899568</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>(125, 4875)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>[-2.24695086 -2.04684412 -2.00907616 ...  4.70365302  5.09968474
+  5.33792856]</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v>5000</v>
+      </c>
+      <c r="R3" t="n">
+        <v>12345</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.5154</v>
+      </c>
+      <c r="T3" t="n">
+        <v>5000</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.65234375</v>
+      </c>
+      <c r="V3" t="n">
+        <v>18</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.4604991813964153</v>
+      </c>
+      <c r="X3" t="n">
+        <v>-0.7752356862657116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>control</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>control_N</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>test_N</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>effect_size</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>is_paired</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
+        <is>
+          <t>difference</t>
+        </is>
+      </c>
+      <c r="I1" s="3" t="inlineStr">
+        <is>
+          <t>ci</t>
+        </is>
+      </c>
+      <c r="J1" s="3" t="inlineStr">
+        <is>
+          <t>bca_low</t>
+        </is>
+      </c>
+      <c r="K1" s="3" t="inlineStr">
+        <is>
+          <t>bca_high</t>
+        </is>
+      </c>
+      <c r="L1" s="3" t="inlineStr">
+        <is>
+          <t>bca_interval_idx</t>
+        </is>
+      </c>
+      <c r="M1" s="3" t="inlineStr">
+        <is>
+          <t>pct_low</t>
+        </is>
+      </c>
+      <c r="N1" s="3" t="inlineStr">
+        <is>
+          <t>pct_high</t>
+        </is>
+      </c>
+      <c r="O1" s="3" t="inlineStr">
+        <is>
+          <t>pct_interval_idx</t>
+        </is>
+      </c>
+      <c r="P1" s="3" t="inlineStr">
+        <is>
+          <t>bootstraps</t>
+        </is>
+      </c>
+      <c r="Q1" s="3" t="inlineStr">
+        <is>
+          <t>resamples</t>
+        </is>
+      </c>
+      <c r="R1" s="3" t="inlineStr">
+        <is>
+          <t>random_seed</t>
+        </is>
+      </c>
+      <c r="S1" s="3" t="inlineStr">
+        <is>
+          <t>pvalue_permutation</t>
+        </is>
+      </c>
+      <c r="T1" s="3" t="inlineStr">
+        <is>
+          <t>permutation_count</t>
+        </is>
+      </c>
+      <c r="U1" s="3" t="inlineStr">
+        <is>
+          <t>pvalue_wilcoxon</t>
+        </is>
+      </c>
+      <c r="V1" s="3" t="inlineStr">
+        <is>
+          <t>statistic_wilcoxon</t>
+        </is>
+      </c>
+      <c r="W1" s="3" t="inlineStr">
+        <is>
+          <t>pvalue_paired_students_t</t>
+        </is>
+      </c>
+      <c r="X1" s="3" t="inlineStr">
+        <is>
+          <t>statistic_paired_students_t</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>control1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>test1</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>mean difference</t>
+        </is>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.181398634009704</v>
+      </c>
+      <c r="I2" t="n">
+        <v>95</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.6080379091540522</v>
+      </c>
+      <c r="K2" t="n">
+        <v>2.535525662759842</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>(74, 4810)</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>-0.4407462515386924</v>
+      </c>
+      <c r="N2" t="n">
+        <v>2.658289886448642</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>(125, 4875)</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>[-1.80529007 -1.80529007 -1.67246845 ...  3.45470257  3.58752419
+  3.66338636]</t>
+        </is>
+      </c>
+      <c r="Q2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="R2" t="n">
+        <v>12345</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.2252</v>
+      </c>
+      <c r="T2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.3125</v>
+      </c>
+      <c r="V2" t="n">
+        <v>5</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.2255779037553131</v>
+      </c>
+      <c r="X2" t="n">
+        <v>-1.381818993572075</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>control2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>test2</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>mean difference</t>
+        </is>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.8396280075262637</v>
+      </c>
+      <c r="I3" t="n">
+        <v>95</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-0.7019448623986144</v>
+      </c>
+      <c r="K3" t="n">
+        <v>3.5002453177765</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>(258, 4956)</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>-0.9379203764316902</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2.978988898899568</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>(125, 4875)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>[-2.24695086 -2.04684412 -2.00907616 ...  4.70365302  5.09968474
+  5.33792856]</t>
+        </is>
+      </c>
+      <c r="Q3" t="n">
+        <v>5000</v>
+      </c>
+      <c r="R3" t="n">
+        <v>12345</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.5154</v>
+      </c>
+      <c r="T3" t="n">
+        <v>5000</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.65234375</v>
+      </c>
+      <c r="V3" t="n">
+        <v>18</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0.4604991813964153</v>
+      </c>
+      <c r="X3" t="n">
+        <v>-0.7752356862657116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -6707,7 +8028,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -7017,7 +8338,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -7327,7 +8648,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -7550,7 +8871,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -7773,7 +9094,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -7996,6 +9317,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>